<commit_message>
after updates for SE domain
</commit_message>
<xml_diff>
--- a/TDF_PSch_ReleaseNotes.xlsx
+++ b/TDF_PSch_ReleaseNotes.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Details" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Details!$A$1:$M$149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Details!$A$1:$M$83</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="248">
   <si>
     <t>Pinnacle 21 ID</t>
   </si>
@@ -693,30 +693,9 @@
     <t>Add missing parameter, searched for value in NDF-RT</t>
   </si>
   <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>VISITNUM</t>
-  </si>
-  <si>
-    <t>SD1076</t>
-  </si>
-  <si>
-    <t>FDAC031</t>
-  </si>
-  <si>
-    <t>Model permissible variable added into standard domain</t>
-  </si>
-  <si>
-    <t>VISIT</t>
-  </si>
-  <si>
     <t>VARIABLE, DATASET</t>
   </si>
   <si>
-    <t>EPOCH, DS</t>
-  </si>
-  <si>
     <t>SD1077</t>
   </si>
   <si>
@@ -726,75 +705,6 @@
     <t>FDA Expected variable EPOCH not found</t>
   </si>
   <si>
-    <t>DSDY</t>
-  </si>
-  <si>
-    <t>SD1083</t>
-  </si>
-  <si>
-    <t>FDAC124</t>
-  </si>
-  <si>
-    <t>Missing DSDY variable, when DSDTC variable is present</t>
-  </si>
-  <si>
-    <t>DSCAT, DSDECOD</t>
-  </si>
-  <si>
-    <t>DISPOSITION EVENT, PROTOCOL VIOLATION</t>
-  </si>
-  <si>
-    <t>DSDECOD value not found in 'Completion/Reason for Non-Completion' extensible codelist when DSCAT == 'DISPOSITION EVENT'</t>
-  </si>
-  <si>
-    <t>DSSPID</t>
-  </si>
-  <si>
-    <t>[1 spaces]7</t>
-  </si>
-  <si>
-    <t>SD1021</t>
-  </si>
-  <si>
-    <t>FDAC216</t>
-  </si>
-  <si>
-    <t>Unexpected character value in DSSPID variable</t>
-  </si>
-  <si>
-    <t>[1 spaces]8</t>
-  </si>
-  <si>
-    <t>[1 spaces]1</t>
-  </si>
-  <si>
-    <t>[1 spaces]9</t>
-  </si>
-  <si>
-    <t>[1 spaces]5</t>
-  </si>
-  <si>
-    <t>[1 spaces]3</t>
-  </si>
-  <si>
-    <t>[1 spaces]6</t>
-  </si>
-  <si>
-    <t>[1 spaces]4</t>
-  </si>
-  <si>
-    <t>[1 spaces]2</t>
-  </si>
-  <si>
-    <t>VISIT, 2</t>
-  </si>
-  <si>
-    <t>DSDTC, 3</t>
-  </si>
-  <si>
-    <t>DSDECOD, 36</t>
-  </si>
-  <si>
     <t>SE</t>
   </si>
   <si>
@@ -831,24 +741,9 @@
     <t>ETCD, 194</t>
   </si>
   <si>
-    <t>remove the blank</t>
-  </si>
-  <si>
     <t>Add EPOCH</t>
   </si>
   <si>
-    <t>check for values in controlled terminology</t>
-  </si>
-  <si>
-    <t>Add DSDY</t>
-  </si>
-  <si>
-    <t>Add SESTDY</t>
-  </si>
-  <si>
-    <t>Add SEENDY</t>
-  </si>
-  <si>
     <t>SUPPDM</t>
   </si>
   <si>
@@ -862,6 +757,14 @@
   </si>
   <si>
     <t>QEVAL, 178</t>
+  </si>
+  <si>
+    <t>Add SESTDY and calculate the value from RFSTDTC (DM) and SESTDTC
+There is a remaining Warning, about an added non-standard variable: P21 make up your mind!!!</t>
+  </si>
+  <si>
+    <t>Add SEENDY and calculate the value from RFSTDTC (DM) and SEENDTC
+There is a remaining Warning, about an added non-standard variable: P21 make up your mind!!!</t>
   </si>
 </sst>
 </file>
@@ -1268,14 +1171,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:M149"/>
+  <dimension ref="A1:M83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H155" sqref="H155"/>
+      <selection pane="bottomRight" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1337,7 +1239,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A2" s="5" t="s">
         <v>89</v>
       </c>
@@ -1374,7 +1276,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="3" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A3" s="5" t="s">
         <v>89</v>
       </c>
@@ -1411,7 +1313,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="4" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A4" s="5" t="s">
         <v>89</v>
       </c>
@@ -1448,7 +1350,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="5" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A5" s="5" t="s">
         <v>89</v>
       </c>
@@ -1485,7 +1387,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="6" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A6" s="5" t="s">
         <v>89</v>
       </c>
@@ -1522,7 +1424,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="7" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A7" s="5" t="s">
         <v>89</v>
       </c>
@@ -1559,7 +1461,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="8" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A8" s="5" t="s">
         <v>89</v>
       </c>
@@ -1596,7 +1498,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="9" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A9" s="5" t="s">
         <v>89</v>
       </c>
@@ -1635,7 +1537,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="10" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A10" s="5" t="s">
         <v>89</v>
       </c>
@@ -1674,7 +1576,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="11" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A11" s="5" t="s">
         <v>89</v>
       </c>
@@ -1713,7 +1615,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="12" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A12" s="5" t="s">
         <v>89</v>
       </c>
@@ -1752,7 +1654,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="13" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A13" s="5" t="s">
         <v>89</v>
       </c>
@@ -1791,7 +1693,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="14" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A14" s="5" t="s">
         <v>89</v>
       </c>
@@ -1830,7 +1732,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="15" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A15" s="5" t="s">
         <v>89</v>
       </c>
@@ -1869,7 +1771,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="16" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A16" s="5" t="s">
         <v>89</v>
       </c>
@@ -1908,7 +1810,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="17" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A17" s="5" t="s">
         <v>89</v>
       </c>
@@ -1947,7 +1849,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="18" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A18" s="5" t="s">
         <v>89</v>
       </c>
@@ -1986,7 +1888,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="19" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A19" s="5" t="s">
         <v>89</v>
       </c>
@@ -2025,7 +1927,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="20" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A20" s="5" t="s">
         <v>89</v>
       </c>
@@ -2064,7 +1966,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="21" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A21" s="5" t="s">
         <v>100</v>
       </c>
@@ -2101,7 +2003,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="22" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A22" s="5" t="s">
         <v>100</v>
       </c>
@@ -2140,7 +2042,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="4" customFormat="1" ht="45" hidden="1">
+    <row r="23" spans="1:13" s="4" customFormat="1" ht="45">
       <c r="A23" s="5" t="s">
         <v>100</v>
       </c>
@@ -2179,7 +2081,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="24" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A24" s="5" t="s">
         <v>100</v>
       </c>
@@ -2216,7 +2118,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="25" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A25" s="5" t="s">
         <v>100</v>
       </c>
@@ -2253,7 +2155,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="26" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A26" s="5" t="s">
         <v>100</v>
       </c>
@@ -2290,7 +2192,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="27" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A27" s="5" t="s">
         <v>100</v>
       </c>
@@ -2327,7 +2229,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="28" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A28" s="5" t="s">
         <v>100</v>
       </c>
@@ -2364,7 +2266,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="4" customFormat="1" ht="60" hidden="1">
+    <row r="29" spans="1:13" s="4" customFormat="1" ht="60">
       <c r="A29" s="4" t="s">
         <v>100</v>
       </c>
@@ -2390,7 +2292,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="30" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A30" s="5" t="s">
         <v>112</v>
       </c>
@@ -2427,7 +2329,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="31" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A31" s="5" t="s">
         <v>112</v>
       </c>
@@ -2464,7 +2366,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="32" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A32" s="5" t="s">
         <v>112</v>
       </c>
@@ -2501,7 +2403,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="33" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A33" s="5" t="s">
         <v>112</v>
       </c>
@@ -2538,7 +2440,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="34" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A34" s="5" t="s">
         <v>112</v>
       </c>
@@ -2575,7 +2477,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="4" customFormat="1" ht="25.5" hidden="1">
+    <row r="35" spans="1:13" s="4" customFormat="1" ht="25.5">
       <c r="A35" s="5" t="s">
         <v>116</v>
       </c>
@@ -2612,7 +2514,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="36" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A36" s="5" t="s">
         <v>116</v>
       </c>
@@ -2649,7 +2551,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="2" customFormat="1" ht="26.25" hidden="1">
+    <row r="37" spans="1:13" s="2" customFormat="1" ht="26.25">
       <c r="A37" s="1" t="s">
         <v>120</v>
       </c>
@@ -2686,7 +2588,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="2" customFormat="1" ht="26.25" hidden="1">
+    <row r="38" spans="1:13" s="2" customFormat="1" ht="26.25">
       <c r="A38" s="1" t="s">
         <v>120</v>
       </c>
@@ -2723,7 +2625,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="2" customFormat="1" ht="26.25" hidden="1">
+    <row r="39" spans="1:13" s="2" customFormat="1" ht="26.25">
       <c r="A39" s="1" t="s">
         <v>120</v>
       </c>
@@ -2760,7 +2662,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="51" hidden="1">
+    <row r="40" spans="1:13" ht="51">
       <c r="A40" s="9" t="s">
         <v>120</v>
       </c>
@@ -2799,7 +2701,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="51" hidden="1">
+    <row r="41" spans="1:13" ht="51">
       <c r="A41" s="9" t="s">
         <v>120</v>
       </c>
@@ -2838,7 +2740,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="2" customFormat="1" ht="51.75" hidden="1">
+    <row r="42" spans="1:13" s="2" customFormat="1" ht="51.75">
       <c r="A42" s="1" t="s">
         <v>120</v>
       </c>
@@ -2877,7 +2779,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="2" customFormat="1" ht="51.75" hidden="1">
+    <row r="43" spans="1:13" s="2" customFormat="1" ht="51.75">
       <c r="A43" s="1" t="s">
         <v>120</v>
       </c>
@@ -2916,7 +2818,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="44" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A44" s="5" t="s">
         <v>120</v>
       </c>
@@ -2953,7 +2855,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="45" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A45" s="5" t="s">
         <v>120</v>
       </c>
@@ -2990,7 +2892,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="46" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A46" s="5" t="s">
         <v>120</v>
       </c>
@@ -3027,7 +2929,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="2" customFormat="1" ht="30" hidden="1">
+    <row r="47" spans="1:13" s="2" customFormat="1" ht="30">
       <c r="A47" s="1" t="s">
         <v>120</v>
       </c>
@@ -3066,7 +2968,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="2" customFormat="1" ht="26.25" hidden="1">
+    <row r="48" spans="1:13" s="2" customFormat="1" ht="26.25">
       <c r="A48" s="1" t="s">
         <v>120</v>
       </c>
@@ -3102,7 +3004,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="2" customFormat="1" ht="26.25" hidden="1">
+    <row r="49" spans="1:13" s="2" customFormat="1" ht="26.25">
       <c r="A49" s="1" t="s">
         <v>120</v>
       </c>
@@ -3138,7 +3040,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="30" hidden="1">
+    <row r="50" spans="1:13" ht="30">
       <c r="A50" s="9" t="s">
         <v>120</v>
       </c>
@@ -3175,7 +3077,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="105" hidden="1">
+    <row r="51" spans="1:13" ht="105">
       <c r="A51" s="9" t="s">
         <v>120</v>
       </c>
@@ -3212,7 +3114,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="60" hidden="1">
+    <row r="52" spans="1:13" ht="60">
       <c r="A52" s="9" t="s">
         <v>120</v>
       </c>
@@ -3249,7 +3151,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="30" hidden="1">
+    <row r="53" spans="1:13" ht="30">
       <c r="A53" s="9" t="s">
         <v>120</v>
       </c>
@@ -3286,7 +3188,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="2" customFormat="1" ht="30" hidden="1">
+    <row r="54" spans="1:13" s="2" customFormat="1" ht="30">
       <c r="A54" s="1" t="s">
         <v>120</v>
       </c>
@@ -3323,7 +3225,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="2" customFormat="1" ht="26.25" hidden="1">
+    <row r="55" spans="1:13" s="2" customFormat="1" ht="26.25">
       <c r="A55" s="1" t="s">
         <v>120</v>
       </c>
@@ -3360,7 +3262,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="30" hidden="1">
+    <row r="56" spans="1:13" ht="30">
       <c r="A56" s="9" t="s">
         <v>120</v>
       </c>
@@ -3397,7 +3299,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="30" hidden="1">
+    <row r="57" spans="1:13" ht="30">
       <c r="A57" s="9" t="s">
         <v>120</v>
       </c>
@@ -3434,7 +3336,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="58" spans="1:13" s="2" customFormat="1" ht="26.25" hidden="1">
+    <row r="58" spans="1:13" s="2" customFormat="1" ht="26.25">
       <c r="A58" s="1" t="s">
         <v>120</v>
       </c>
@@ -3471,7 +3373,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="2" customFormat="1" ht="26.25" hidden="1">
+    <row r="59" spans="1:13" s="2" customFormat="1" ht="26.25">
       <c r="A59" s="1" t="s">
         <v>120</v>
       </c>
@@ -3508,7 +3410,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="60" spans="1:13" s="2" customFormat="1" ht="26.25" hidden="1">
+    <row r="60" spans="1:13" s="2" customFormat="1" ht="26.25">
       <c r="A60" s="1" t="s">
         <v>120</v>
       </c>
@@ -3545,7 +3447,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:13" s="2" customFormat="1" ht="26.25" hidden="1">
+    <row r="61" spans="1:13" s="2" customFormat="1" ht="26.25">
       <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
@@ -3582,7 +3484,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="2" customFormat="1" ht="26.25" hidden="1">
+    <row r="62" spans="1:13" s="2" customFormat="1" ht="26.25">
       <c r="A62" s="1" t="s">
         <v>120</v>
       </c>
@@ -3619,7 +3521,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="2" customFormat="1" ht="26.25" hidden="1">
+    <row r="63" spans="1:13" s="2" customFormat="1" ht="26.25">
       <c r="A63" s="1" t="s">
         <v>120</v>
       </c>
@@ -3656,7 +3558,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="2" customFormat="1" ht="60" hidden="1">
+    <row r="64" spans="1:13" s="2" customFormat="1" ht="60">
       <c r="A64" s="1" t="s">
         <v>120</v>
       </c>
@@ -3695,7 +3597,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:13" s="4" customFormat="1" ht="60" hidden="1">
+    <row r="65" spans="1:13" s="4" customFormat="1" ht="60">
       <c r="A65" s="5" t="s">
         <v>161</v>
       </c>
@@ -3732,7 +3634,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="66" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A66" s="5" t="s">
         <v>161</v>
       </c>
@@ -3769,7 +3671,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="67" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A67" s="5" t="s">
         <v>161</v>
       </c>
@@ -3806,7 +3708,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="68" spans="1:13" s="4" customFormat="1" ht="30" hidden="1">
+    <row r="68" spans="1:13" s="4" customFormat="1" ht="30">
       <c r="A68" s="5" t="s">
         <v>161</v>
       </c>
@@ -3843,7 +3745,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="36" hidden="1" customHeight="1">
+    <row r="69" spans="1:13" ht="36" customHeight="1">
       <c r="A69" s="9" t="s">
         <v>120</v>
       </c>
@@ -3880,7 +3782,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="13" customFormat="1" ht="45" hidden="1">
+    <row r="70" spans="1:13" s="13" customFormat="1" ht="45">
       <c r="A70" s="11" t="s">
         <v>120</v>
       </c>
@@ -3919,7 +3821,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="71" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
+    <row r="71" spans="1:13" s="13" customFormat="1" ht="25.5">
       <c r="A71" s="11" t="s">
         <v>120</v>
       </c>
@@ -3958,7 +3860,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="72" spans="1:13" s="13" customFormat="1" ht="75" hidden="1">
+    <row r="72" spans="1:13" s="13" customFormat="1" ht="75">
       <c r="A72" s="11" t="s">
         <v>120</v>
       </c>
@@ -3997,7 +3899,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="73" spans="1:13" s="13" customFormat="1" ht="30" hidden="1">
+    <row r="73" spans="1:13" s="13" customFormat="1" ht="30">
       <c r="A73" s="11" t="s">
         <v>120</v>
       </c>
@@ -4036,26 +3938,26 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
+    <row r="74" spans="1:13" s="13" customFormat="1" ht="25.5">
       <c r="A74" s="9" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9" t="s">
-        <v>121</v>
+        <v>224</v>
       </c>
       <c r="E74" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="F74" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="F74" s="14" t="s">
+      <c r="G74" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="G74" s="14" t="s">
+      <c r="H74" s="9" t="s">
         <v>227</v>
-      </c>
-      <c r="H74" s="9" t="s">
-        <v>228</v>
       </c>
       <c r="I74" s="9" t="s">
         <v>15</v>
@@ -4063,13 +3965,19 @@
       <c r="J74" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L74" s="9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
+      <c r="K74" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="L74" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="M74" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="75">
       <c r="A75" s="9" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -4077,2696 +3985,334 @@
         <v>121</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="G75" s="9" t="s">
-        <v>227</v>
+        <v>230</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>232</v>
       </c>
       <c r="H75" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="I75" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J75" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K75" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="L75" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M75" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="75">
+      <c r="A76" s="9" t="s">
         <v>228</v>
-      </c>
-      <c r="I75" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J75" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L75" s="9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A76" s="9" t="s">
-        <v>224</v>
       </c>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9" t="s">
-        <v>230</v>
+        <v>121</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="F76" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="G76" s="14" t="s">
-        <v>233</v>
+        <v>234</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>236</v>
       </c>
       <c r="H76" s="9" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="I76" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J76" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K76" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="L76" s="9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" s="13" customFormat="1" ht="38.25" hidden="1">
+        <v>6</v>
+      </c>
+      <c r="K76" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="L76" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M76" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" s="13" customFormat="1" ht="30">
       <c r="A77" s="9" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
       <c r="D77" s="9" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>235</v>
+        <v>110</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>236</v>
+        <v>24</v>
       </c>
       <c r="G77" s="14" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="H77" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I77" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J77" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K77" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="L77" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M77" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" s="13" customFormat="1" ht="30">
+      <c r="A78" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E78" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="I77" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J77" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K77" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="L77" s="9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" s="13" customFormat="1" ht="63.75" hidden="1">
-      <c r="A78" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9">
-        <v>6</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="F78" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G78" s="14" t="s">
-        <v>11</v>
+      <c r="F78" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>241</v>
+        <v>26</v>
       </c>
       <c r="I78" s="9" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J78" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K78" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="L78" s="9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
+        <v>6</v>
+      </c>
+      <c r="K78" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="L78" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M78" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" s="13" customFormat="1" ht="30">
       <c r="A79" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B79" s="9">
-        <v>40</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="B79" s="9"/>
       <c r="C79" s="9"/>
       <c r="D79" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H79" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I79" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J79" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K79" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="L79" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M79" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" customFormat="1" ht="30">
+      <c r="A80" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E79" s="9" t="s">
+      <c r="F80" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G80" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K80" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="L80" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M80" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" customFormat="1" ht="30">
+      <c r="A81" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F79" s="14" t="s">
+      <c r="F81" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K81" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="L81" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M81" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" customFormat="1" ht="30">
+      <c r="A82" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="G79" s="14" t="s">
+      <c r="F82" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K82" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="L82" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M82" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" customFormat="1" ht="30">
+      <c r="A83" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="H79" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I79" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J79" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K79" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L79" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A80" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B80" s="9">
-        <v>109</v>
-      </c>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G80" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H80" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I80" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J80" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K80" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L80" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A81" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B81" s="9">
-        <v>111</v>
-      </c>
-      <c r="C81" s="9"/>
-      <c r="D81" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G81" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H81" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I81" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J81" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K81" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L81" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A82" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B82" s="9">
-        <v>123</v>
-      </c>
-      <c r="C82" s="9"/>
-      <c r="D82" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G82" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H82" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I82" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J82" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K82" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L82" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A83" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B83" s="9">
-        <v>142</v>
-      </c>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G83" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H83" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I83" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J83" s="9" t="s">
-        <v>9</v>
+      <c r="F83" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="K83" s="8" t="s">
-        <v>270</v>
+        <v>167</v>
       </c>
       <c r="L83" s="8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A84" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B84" s="9">
-        <v>146</v>
-      </c>
-      <c r="C84" s="9"/>
-      <c r="D84" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G84" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H84" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I84" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J84" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K84" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L84" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A85" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B85" s="9">
-        <v>154</v>
-      </c>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G85" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H85" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I85" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J85" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K85" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L85" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A86" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B86" s="9">
-        <v>160</v>
-      </c>
-      <c r="C86" s="9"/>
-      <c r="D86" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="F86" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G86" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H86" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I86" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J86" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K86" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L86" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A87" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B87" s="9">
-        <v>165</v>
-      </c>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G87" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H87" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I87" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J87" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K87" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L87" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A88" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B88" s="9">
-        <v>177</v>
-      </c>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G88" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H88" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I88" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J88" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K88" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L88" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A89" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B89" s="9">
-        <v>187</v>
-      </c>
-      <c r="C89" s="9"/>
-      <c r="D89" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G89" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H89" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I89" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J89" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K89" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L89" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A90" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B90" s="9">
-        <v>195</v>
-      </c>
-      <c r="C90" s="9"/>
-      <c r="D90" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E90" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="F90" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G90" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H90" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I90" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K90" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L90" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A91" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B91" s="9">
-        <v>203</v>
-      </c>
-      <c r="C91" s="9"/>
-      <c r="D91" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F91" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G91" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H91" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I91" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J91" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K91" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L91" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A92" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B92" s="9">
-        <v>209</v>
-      </c>
-      <c r="C92" s="9"/>
-      <c r="D92" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="F92" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G92" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H92" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I92" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J92" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K92" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L92" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A93" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B93" s="9">
-        <v>214</v>
-      </c>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="F93" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G93" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H93" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I93" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J93" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K93" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L93" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A94" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B94" s="9">
-        <v>220</v>
-      </c>
-      <c r="C94" s="9"/>
-      <c r="D94" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F94" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G94" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H94" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I94" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J94" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K94" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L94" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A95" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B95" s="9">
-        <v>222</v>
-      </c>
-      <c r="C95" s="9"/>
-      <c r="D95" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G95" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H95" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I95" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J95" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K95" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L95" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A96" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B96" s="9">
-        <v>230</v>
-      </c>
-      <c r="C96" s="9"/>
-      <c r="D96" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E96" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F96" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G96" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H96" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I96" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J96" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K96" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L96" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A97" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B97" s="9">
-        <v>237</v>
-      </c>
-      <c r="C97" s="9"/>
-      <c r="D97" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="F97" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G97" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H97" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I97" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J97" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K97" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L97" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A98" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B98" s="9">
-        <v>251</v>
-      </c>
-      <c r="C98" s="9"/>
-      <c r="D98" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E98" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F98" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G98" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H98" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I98" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J98" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K98" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L98" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A99" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B99" s="9">
-        <v>253</v>
-      </c>
-      <c r="C99" s="9"/>
-      <c r="D99" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E99" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G99" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H99" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I99" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J99" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K99" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L99" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A100" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B100" s="9">
-        <v>262</v>
-      </c>
-      <c r="C100" s="9"/>
-      <c r="D100" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E100" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="F100" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G100" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H100" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I100" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J100" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K100" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L100" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A101" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B101" s="9">
-        <v>269</v>
-      </c>
-      <c r="C101" s="9"/>
-      <c r="D101" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G101" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H101" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I101" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J101" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K101" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L101" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A102" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B102" s="9">
-        <v>271</v>
-      </c>
-      <c r="C102" s="9"/>
-      <c r="D102" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E102" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="F102" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G102" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H102" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I102" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J102" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K102" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L102" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A103" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B103" s="9">
-        <v>284</v>
-      </c>
-      <c r="C103" s="9"/>
-      <c r="D103" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G103" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H103" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I103" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J103" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K103" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L103" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A104" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B104" s="9">
-        <v>292</v>
-      </c>
-      <c r="C104" s="9"/>
-      <c r="D104" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E104" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="F104" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G104" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H104" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I104" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J104" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K104" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L104" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A105" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B105" s="9">
-        <v>297</v>
-      </c>
-      <c r="C105" s="9"/>
-      <c r="D105" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E105" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="F105" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G105" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H105" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I105" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J105" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K105" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L105" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A106" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B106" s="9">
-        <v>305</v>
-      </c>
-      <c r="C106" s="9"/>
-      <c r="D106" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E106" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="F106" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G106" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H106" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I106" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J106" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K106" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L106" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A107" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B107" s="9">
-        <v>309</v>
-      </c>
-      <c r="C107" s="9"/>
-      <c r="D107" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E107" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="F107" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G107" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H107" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I107" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J107" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K107" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L107" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A108" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B108" s="9">
-        <v>315</v>
-      </c>
-      <c r="C108" s="9"/>
-      <c r="D108" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="F108" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G108" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H108" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I108" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J108" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K108" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L108" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A109" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B109" s="9">
-        <v>321</v>
-      </c>
-      <c r="C109" s="9"/>
-      <c r="D109" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="F109" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G109" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H109" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I109" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J109" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K109" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L109" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A110" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B110" s="9">
-        <v>323</v>
-      </c>
-      <c r="C110" s="9"/>
-      <c r="D110" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F110" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G110" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H110" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I110" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J110" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K110" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L110" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A111" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B111" s="9">
-        <v>329</v>
-      </c>
-      <c r="C111" s="9"/>
-      <c r="D111" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E111" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="F111" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G111" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H111" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I111" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J111" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K111" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L111" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A112" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B112" s="9">
-        <v>337</v>
-      </c>
-      <c r="C112" s="9"/>
-      <c r="D112" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E112" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F112" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G112" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H112" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I112" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J112" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K112" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L112" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A113" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B113" s="9">
-        <v>349</v>
-      </c>
-      <c r="C113" s="9"/>
-      <c r="D113" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E113" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="F113" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G113" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H113" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I113" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J113" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K113" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L113" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A114" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B114" s="9">
-        <v>351</v>
-      </c>
-      <c r="C114" s="9"/>
-      <c r="D114" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E114" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F114" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G114" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H114" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I114" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J114" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K114" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L114" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A115" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B115" s="9">
-        <v>355</v>
-      </c>
-      <c r="C115" s="9"/>
-      <c r="D115" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E115" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="F115" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G115" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H115" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I115" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J115" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K115" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L115" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A116" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B116" s="9">
-        <v>359</v>
-      </c>
-      <c r="C116" s="9"/>
-      <c r="D116" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E116" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="F116" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G116" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H116" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I116" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J116" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K116" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L116" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A117" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B117" s="9">
-        <v>361</v>
-      </c>
-      <c r="C117" s="9"/>
-      <c r="D117" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E117" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="F117" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G117" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H117" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I117" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J117" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K117" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L117" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A118" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B118" s="9">
-        <v>371</v>
-      </c>
-      <c r="C118" s="9"/>
-      <c r="D118" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E118" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F118" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G118" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H118" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I118" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J118" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K118" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L118" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A119" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B119" s="9">
-        <v>374</v>
-      </c>
-      <c r="C119" s="9"/>
-      <c r="D119" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E119" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="F119" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G119" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H119" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I119" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J119" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K119" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L119" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A120" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B120" s="9">
-        <v>376</v>
-      </c>
-      <c r="C120" s="9"/>
-      <c r="D120" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E120" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="F120" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G120" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H120" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I120" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J120" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K120" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L120" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A121" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B121" s="9">
-        <v>379</v>
-      </c>
-      <c r="C121" s="9"/>
-      <c r="D121" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E121" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="F121" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G121" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H121" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I121" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J121" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K121" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L121" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A122" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B122" s="9">
-        <v>394</v>
-      </c>
-      <c r="C122" s="9"/>
-      <c r="D122" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E122" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="F122" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G122" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H122" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I122" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J122" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K122" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L122" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A123" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B123" s="9">
-        <v>400</v>
-      </c>
-      <c r="C123" s="9"/>
-      <c r="D123" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E123" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="F123" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G123" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H123" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I123" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J123" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K123" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L123" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A124" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B124" s="9">
-        <v>404</v>
-      </c>
-      <c r="C124" s="9"/>
-      <c r="D124" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E124" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F124" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G124" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H124" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I124" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J124" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K124" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L124" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A125" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B125" s="9">
-        <v>420</v>
-      </c>
-      <c r="C125" s="9"/>
-      <c r="D125" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E125" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="F125" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G125" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H125" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I125" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J125" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K125" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L125" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A126" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B126" s="9">
-        <v>444</v>
-      </c>
-      <c r="C126" s="9"/>
-      <c r="D126" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E126" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F126" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G126" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H126" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I126" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J126" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K126" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L126" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="127" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A127" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B127" s="9">
-        <v>454</v>
-      </c>
-      <c r="C127" s="9"/>
-      <c r="D127" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E127" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="F127" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G127" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H127" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I127" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J127" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K127" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L127" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="128" spans="1:12" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A128" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B128" s="9">
-        <v>459</v>
-      </c>
-      <c r="C128" s="9"/>
-      <c r="D128" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E128" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="F128" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G128" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H128" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I128" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J128" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K128" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L128" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="129" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A129" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B129" s="9">
-        <v>471</v>
-      </c>
-      <c r="C129" s="9"/>
-      <c r="D129" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E129" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="F129" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G129" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H129" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I129" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J129" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K129" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L129" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="130" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A130" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B130" s="9">
-        <v>482</v>
-      </c>
-      <c r="C130" s="9"/>
-      <c r="D130" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E130" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F130" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G130" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H130" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I130" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J130" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K130" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L130" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="131" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A131" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B131" s="9">
-        <v>487</v>
-      </c>
-      <c r="C131" s="9"/>
-      <c r="D131" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E131" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F131" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G131" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H131" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I131" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J131" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K131" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L131" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="132" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A132" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B132" s="9">
-        <v>514</v>
-      </c>
-      <c r="C132" s="9"/>
-      <c r="D132" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E132" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F132" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G132" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H132" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I132" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J132" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K132" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L132" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="133" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A133" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B133" s="9">
-        <v>528</v>
-      </c>
-      <c r="C133" s="9"/>
-      <c r="D133" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E133" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="F133" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G133" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H133" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I133" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J133" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K133" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L133" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="134" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A134" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B134" s="9">
-        <v>543</v>
-      </c>
-      <c r="C134" s="9"/>
-      <c r="D134" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E134" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F134" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G134" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H134" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I134" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J134" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K134" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L134" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="135" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A135" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B135" s="9">
-        <v>567</v>
-      </c>
-      <c r="C135" s="9"/>
-      <c r="D135" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E135" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="F135" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G135" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H135" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I135" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J135" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K135" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L135" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="136" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A136" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B136" s="9">
-        <v>582</v>
-      </c>
-      <c r="C136" s="9"/>
-      <c r="D136" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E136" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="F136" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G136" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H136" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="I136" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J136" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K136" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="L136" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="137" spans="1:13" s="13" customFormat="1" ht="30" hidden="1">
-      <c r="A137" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B137" s="9"/>
-      <c r="C137" s="9"/>
-      <c r="D137" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E137" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="F137" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G137" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H137" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I137" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J137" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K137" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="L137" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="138" spans="1:13" s="13" customFormat="1" ht="30" hidden="1">
-      <c r="A138" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B138" s="9"/>
-      <c r="C138" s="9"/>
-      <c r="D138" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E138" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="F138" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G138" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H138" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I138" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J138" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K138" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="L138" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="139" spans="1:13" s="13" customFormat="1" ht="30" hidden="1">
-      <c r="A139" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B139" s="9"/>
-      <c r="C139" s="9"/>
-      <c r="D139" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E139" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="F139" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G139" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H139" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I139" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J139" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K139" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="L139" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="140" spans="1:13" s="13" customFormat="1" ht="25.5" hidden="1">
-      <c r="A140" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="B140" s="9"/>
-      <c r="C140" s="9"/>
-      <c r="D140" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="E140" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="F140" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="G140" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="H140" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="I140" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J140" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K140" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="L140" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="M140" s="13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="141" spans="1:13" s="13" customFormat="1" ht="38.25">
-      <c r="A141" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="B141" s="9"/>
-      <c r="C141" s="9"/>
-      <c r="D141" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E141" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="F141" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="G141" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="H141" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="I141" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J141" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K141" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="L141" s="13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="142" spans="1:13" s="13" customFormat="1" ht="38.25">
-      <c r="A142" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="B142" s="9"/>
-      <c r="C142" s="9"/>
-      <c r="D142" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E142" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="F142" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="G142" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="H142" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="I142" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J142" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K142" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="L142" s="13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="143" spans="1:13" s="13" customFormat="1" ht="30" hidden="1">
-      <c r="A143" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="B143" s="9"/>
-      <c r="C143" s="9"/>
-      <c r="D143" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E143" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F143" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G143" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H143" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I143" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J143" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K143" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="L143" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M143" s="13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="144" spans="1:13" s="13" customFormat="1" ht="30" hidden="1">
-      <c r="A144" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="B144" s="9"/>
-      <c r="C144" s="9"/>
-      <c r="D144" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E144" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="F144" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G144" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H144" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I144" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J144" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K144" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="L144" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M144" s="13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="145" spans="1:13" s="13" customFormat="1" ht="30" hidden="1">
-      <c r="A145" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="B145" s="9"/>
-      <c r="C145" s="9"/>
-      <c r="D145" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E145" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="F145" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G145" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H145" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I145" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J145" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K145" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="L145" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M145" s="13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="146" spans="1:13" customFormat="1" ht="30" hidden="1">
-      <c r="A146" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B146" s="1"/>
-      <c r="C146" s="1"/>
-      <c r="D146" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="F146" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G146" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H146" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I146" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J146" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K146" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="L146" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M146" s="13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="147" spans="1:13" customFormat="1" ht="30" hidden="1">
-      <c r="A147" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B147" s="1"/>
-      <c r="C147" s="1"/>
-      <c r="D147" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G147" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H147" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I147" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J147" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K147" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="L147" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M147" s="13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="148" spans="1:13" customFormat="1" ht="30" hidden="1">
-      <c r="A148" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B148" s="1"/>
-      <c r="C148" s="1"/>
-      <c r="D148" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G148" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H148" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I148" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J148" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K148" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="L148" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M148" s="13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="149" spans="1:13" customFormat="1" ht="30" hidden="1">
-      <c r="A149" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B149" s="1"/>
-      <c r="C149" s="1"/>
-      <c r="D149" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F149" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G149" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H149" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I149" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J149" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K149" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="L149" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M149" s="13" t="s">
+      <c r="M83" s="13" t="s">
         <v>173</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M149">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="SE"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:M83">
+    <filterColumn colId="0"/>
     <filterColumn colId="3"/>
-    <filterColumn colId="12">
-      <filters blank="1"/>
-    </filterColumn>
+    <filterColumn colId="12"/>
   </autoFilter>
   <hyperlinks>
     <hyperlink ref="F2" location="'Rules'!A162" display="SD1082"/>
@@ -6851,28 +4397,16 @@
     <hyperlink ref="G73" location="'Rules'!A293" display="FDAC292"/>
     <hyperlink ref="F69" location="'Rules'!A284" display="SD2233"/>
     <hyperlink ref="G69" location="'Rules'!A284" display="FDAC302"/>
-    <hyperlink ref="F74" location="'Rules'!A158" display="SD1076"/>
-    <hyperlink ref="G74" location="'Rules'!A158" display="FDAC031"/>
-    <hyperlink ref="F76" location="'Rules'!A159" display="SD1077"/>
-    <hyperlink ref="G76" location="'Rules'!A159" display="FDAC021"/>
-    <hyperlink ref="F77" location="'Rules'!A163" display="SD1083"/>
-    <hyperlink ref="G77" location="'Rules'!A163" display="FDAC124"/>
-    <hyperlink ref="F78" location="'Rules'!A6" display="CT2005"/>
-    <hyperlink ref="G78" location="'Rules'!A6" display="FDAC344"/>
-    <hyperlink ref="F79" location="'Rules'!A113" display="SD1021"/>
-    <hyperlink ref="G79" location="'Rules'!A113" display="FDAC216"/>
-    <hyperlink ref="F137" location="'Rules'!A162" display="SD1082"/>
-    <hyperlink ref="G137" location="'Rules'!A162" display="FDAC036"/>
-    <hyperlink ref="F140" location="'Rules'!A159" display="SD1077"/>
-    <hyperlink ref="G140" location="'Rules'!A159" display="FDAC021"/>
-    <hyperlink ref="F141" location="'Rules'!A167" display="SD1087"/>
-    <hyperlink ref="G141" location="'Rules'!A167" display="FDAC128"/>
-    <hyperlink ref="F142" location="'Rules'!A171" display="SD1091"/>
-    <hyperlink ref="G142" location="'Rules'!A171" display="FDAC132"/>
-    <hyperlink ref="F143" location="'Rules'!A162" display="SD1082"/>
-    <hyperlink ref="G143" location="'Rules'!A162" display="FDAC036"/>
-    <hyperlink ref="F146" location="'Rules'!A162" display="SD1082"/>
-    <hyperlink ref="G146" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F74" location="'Rules'!A159" display="SD1077"/>
+    <hyperlink ref="G74" location="'Rules'!A159" display="FDAC021"/>
+    <hyperlink ref="F75" location="'Rules'!A167" display="SD1087"/>
+    <hyperlink ref="G75" location="'Rules'!A167" display="FDAC128"/>
+    <hyperlink ref="F76" location="'Rules'!A171" display="SD1091"/>
+    <hyperlink ref="G76" location="'Rules'!A171" display="FDAC132"/>
+    <hyperlink ref="F77" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G77" location="'Rules'!A162" display="FDAC036"/>
+    <hyperlink ref="F80" location="'Rules'!A162" display="SD1082"/>
+    <hyperlink ref="G80" location="'Rules'!A162" display="FDAC036"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>